<commit_message>
Added analysis to test results
</commit_message>
<xml_diff>
--- a/doc/async_test_res.xlsx
+++ b/doc/async_test_res.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82035472-BFCB-439A-80B0-F1A0EC4CA002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E715CE4-1C2F-49BE-AE86-2357F99B68C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2604" windowWidth="25620" windowHeight="12204" xr2:uid="{C987650C-721D-418C-9F6E-6CA2C8470AB6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{C987650C-721D-418C-9F6E-6CA2C8470AB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="24">
   <si>
     <t>p(90) latency</t>
   </si>
@@ -95,13 +95,32 @@
   </si>
   <si>
     <t>error</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>Put</t>
+  </si>
+  <si>
+    <t>Overhead Decrease</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,14 +146,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -446,17 +468,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB0313F-B6B8-461E-A9E7-27471F2F50D7}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A24" sqref="A22:J24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.88671875" customWidth="1"/>
     <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
@@ -1141,6 +1163,402 @@
         <v>129</v>
       </c>
     </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="1">
+        <f>(B3-B2)/B3</f>
+        <v>0.90781755196304847</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" ref="C24:J24" si="0">(C3-C2)/C3</f>
+        <v>-1.5933908045977012</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.88118022328548651</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.1570196078431372</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.29544659718822136</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.5872687578995748</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="1">
+        <f>(B5-B4)/B5</f>
+        <v>0.80960044668516906</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" ref="C25:J25" si="1">(C5-C4)/C5</f>
+        <v>-0.17111459968602824</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="1"/>
+        <v>7.2599531615925084E-2</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="1"/>
+        <v>3.017031630170321E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="1"/>
+        <v>0.23960720130932897</v>
+      </c>
+      <c r="G25" s="1">
+        <f>(G5-G4)/G5</f>
+        <v>-4.0950858969236916E-3</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="1"/>
+        <v>-2.084848484848485</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="1">
+        <f>(B7-B6)/B7</f>
+        <v>0.41419035074010413</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" ref="C26:J26" si="2">(C7-C6)/C7</f>
+        <v>-1.2012012012012022E-2</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.42916093535075672</v>
+      </c>
+      <c r="E26" s="1">
+        <f>(E7-E6)/E7</f>
+        <v>-1.0401691331923888</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="2"/>
+        <v>-6.298533218291634E-2</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="2"/>
+        <v>4.7860629845888772E-3</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.34399999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1">
+        <f>(B10-B9)/B10</f>
+        <v>0.64712499999999995</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" ref="C28:J28" si="3">(C10-C9)/C10</f>
+        <v>-1.4835752482811304</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.30801616705961599</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.53922504294712725</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.13229610544049161</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="3"/>
+        <v>7.2675175827038294E-2</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.2658227848101266E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="1">
+        <f>(B12-B11)/B12</f>
+        <v>8.3928343163930594E-2</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" ref="C29:J29" si="4">(C12-C11)/C12</f>
+        <v>-1.5673981191222656E-2</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="4"/>
+        <v>4.608294930875478E-3</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="4"/>
+        <v>7.2788353863381308E-3</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="4"/>
+        <v>1.5426497277676945E-2</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.6162635485076618E-3</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="4"/>
+        <v>0.18050541516245489</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="1">
+        <f>(B14-B13)/B14</f>
+        <v>0.26129541864139016</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" ref="C30:J30" si="5">(C14-C13)/C14</f>
+        <v>0.3294117647058824</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="5"/>
+        <v>1.7495395948434578E-2</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="5"/>
+        <v>3.3081285444234373E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="5"/>
+        <v>6.7758749069247962E-2</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="5"/>
+        <v>2.9648894668400519E-3</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="5"/>
+        <v>-8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="1">
+        <f>(B17-B16)/B17</f>
+        <v>-1.3607082124637391</v>
+      </c>
+      <c r="C32" s="1">
+        <f t="shared" ref="C32:J32" si="6">(C17-C16)/C17</f>
+        <v>-1.236006051437216</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="6"/>
+        <v>-0.58368336025848144</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="6"/>
+        <v>-0.81912335860921026</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="6"/>
+        <v>-0.45226856757537798</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="6"/>
+        <v>0.16617389125532447</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J32" s="1">
+        <f t="shared" si="6"/>
+        <v>0.23123123123123124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="1">
+        <f>(B19-B18)/B19</f>
+        <v>0.59235052981669112</v>
+      </c>
+      <c r="C33" s="1">
+        <f t="shared" ref="C33:J33" si="7">(C19-C18)/C19</f>
+        <v>0.11129032258064522</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="7"/>
+        <v>9.9064391854705586E-2</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="7"/>
+        <v>8.870967741935494E-2</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="7"/>
+        <v>4.3034605146406342E-2</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.7205781142463867E-2</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="1">
+        <f t="shared" si="7"/>
+        <v>0.10163934426229508</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="1">
+        <f>(B21-B20)/B21</f>
+        <v>-1.0206035310874824</v>
+      </c>
+      <c r="C34" s="1">
+        <f t="shared" ref="C34:J34" si="8">(C21-C20)/C21</f>
+        <v>6.363636363636363E-2</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="8"/>
+        <v>-0.12377560106856622</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="8"/>
+        <v>-8.9445438282647269E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="8"/>
+        <v>-0.30604719764011801</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" si="8"/>
+        <v>1.8278509544269916E-2</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J34" s="1">
+        <f t="shared" si="8"/>
+        <v>2.3255813953488372E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>